<commit_message>
Add new tools folders; Calculate LD and get LD blocks with PLINK
</commit_message>
<xml_diff>
--- a/Data/Parkinsons/Nalls_23andMe/Nalls2019_TableS2.xlsx
+++ b/Data/Parkinsons/Nalls_23andMe/Nalls2019_TableS2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/Parkinsons/Nalls_23andMe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289A9E3B-B29E-814F-A58F-6AB450DC7806}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F414142-4EBE-4D4E-8778-09EB6D5CF4F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="460" windowWidth="21360" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11240" yWindow="460" windowWidth="21360" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tableS2.tab" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="256">
   <si>
     <t>SNP</t>
   </si>
@@ -782,6 +782,12 @@
   </si>
   <si>
     <t>DDRGK1</t>
+  </si>
+  <si>
+    <t>LRRK2_alt</t>
+  </si>
+  <si>
+    <t>LRRK2_rare</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,6 +834,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7A81FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -869,6 +881,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,8 +1207,8 @@
   </sheetPr>
   <dimension ref="A1:AE983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:XFD116"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6694,7 +6707,7 @@
       </c>
     </row>
     <row r="59" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B59" s="1">
@@ -6799,7 +6812,7 @@
         <v>40734202</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>158</v>
+        <v>255</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>158</v>
@@ -10474,7 +10487,7 @@
         <v>40922572</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>158</v>
+        <v>254</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">

</xml_diff>